<commit_message>
Mejoras Receta, hospitalización, servicios
</commit_message>
<xml_diff>
--- a/plantillas/Receta.xlsx
+++ b/plantillas/Receta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorge\Veterinaria\veterinaria-server\plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97952903-6C72-4B02-B465-8B499E1AD6B8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44C64A30-E78B-4E1A-9401-39FB3C87E287}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7425" xr2:uid="{FB37194D-C044-45CF-8888-992560DA2B2F}"/>
   </bookViews>
@@ -303,7 +303,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -326,15 +326,57 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -353,50 +395,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -770,155 +776,156 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{471CDB29-E96B-4EE3-9A11-A23FEEEB5CD9}">
   <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:B7"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="8" width="11.42578125" style="33"/>
+    <col min="9" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="4"/>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="12"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="26"/>
     </row>
     <row r="2" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
+      <c r="A2" s="9"/>
       <c r="B2" s="5"/>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="14"/>
-      <c r="O2" s="9"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="28"/>
+      <c r="O2" s="8"/>
     </row>
     <row r="3" spans="1:15" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6"/>
       <c r="B3" s="7"/>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="16"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="30"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="17" t="s">
+      <c r="B4" s="24"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="18"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="22"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="18"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="19" t="s">
+      <c r="B5" s="16"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="20"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="24"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="20"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="20"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="19" t="s">
+      <c r="B6" s="16"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="20"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="24"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="20"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="19"/>
-      <c r="B7" s="20"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="24"/>
+      <c r="A7" s="15"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="20"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="28"/>
-      <c r="H8" s="28"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
     </row>
     <row r="9" spans="1:15" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A9" s="27"/>
-      <c r="B9" s="27"/>
-      <c r="C9" s="27"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="27"/>
+      <c r="A9" s="10"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
     </row>
     <row r="10" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="29" t="s">
+      <c r="A10" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="31"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="29" t="s">
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="31"/>
-      <c r="G10" s="31"/>
-      <c r="H10" s="30"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="14"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
+      <c r="A11" s="31"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A9:H9"/>
-    <mergeCell ref="B8:H8"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="E10:H10"/>
-    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="C2:H2"/>
+    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="G6:H6"/>
@@ -932,11 +939,11 @@
     <mergeCell ref="E5:F5"/>
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="E7:F7"/>
-    <mergeCell ref="C1:H1"/>
-    <mergeCell ref="C2:H2"/>
-    <mergeCell ref="C3:H3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="B8:H8"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="E10:H10"/>
+    <mergeCell ref="A6:B6"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>